<commit_message>
Created FrontEndplate Grungeplates and added to Front Assembly
</commit_message>
<xml_diff>
--- a/1 1 Front Aerodynamic Devices/FrontEndplate/GenericEndplate.xlsx
+++ b/1 1 Front Aerodynamic Devices/FrontEndplate/GenericEndplate.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="50" yWindow="-40" windowWidth="8910" windowHeight="6680"/>
+    <workbookView visibility="veryHidden" xWindow="50" yWindow="-40" windowWidth="10550" windowHeight="8210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="Family">Sheet1!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1141,12 +1141,12 @@
   <dimension ref="A1:AP12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="AQ2" sqref="AQ2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.90625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" style="1" customWidth="1"/>
     <col min="2" max="3" width="5.7265625" style="27" customWidth="1"/>
     <col min="4" max="4" width="5.7265625" style="29" customWidth="1"/>
     <col min="5" max="5" width="5.7265625" style="33" customWidth="1"/>
@@ -1174,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:42" s="5" customFormat="1" ht="197.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" s="5" customFormat="1" ht="196.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="28" t="s">
         <v>2</v>
@@ -1306,11 +1306,11 @@
       </c>
       <c r="B3" s="27">
         <f>Default!C5</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C3" s="27">
         <f>Default!C6</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D3" s="29">
         <f>Default!C12</f>
@@ -1468,10 +1468,10 @@
         <v>92</v>
       </c>
       <c r="B4" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C4" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4" s="29">
         <v>26</v>
@@ -1597,10 +1597,10 @@
         <v>93</v>
       </c>
       <c r="B5" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C5" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D5" s="29">
         <v>26</v>
@@ -1725,10 +1725,10 @@
         <v>94</v>
       </c>
       <c r="B6" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D6" s="29">
         <v>26</v>
@@ -1853,10 +1853,10 @@
         <v>95</v>
       </c>
       <c r="B7" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C7" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D7" s="29">
         <v>26</v>
@@ -1981,10 +1981,10 @@
         <v>96</v>
       </c>
       <c r="B8" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D8" s="29">
         <v>26</v>
@@ -2109,10 +2109,10 @@
         <v>97</v>
       </c>
       <c r="B9" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C9" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D9" s="29">
         <v>26</v>
@@ -2237,10 +2237,10 @@
         <v>98</v>
       </c>
       <c r="B10" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C10" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D10" s="29">
         <v>26</v>
@@ -2365,10 +2365,10 @@
         <v>99</v>
       </c>
       <c r="B11" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C11" s="27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D11" s="29">
         <v>26</v>
@@ -2512,7 +2512,7 @@
       <c r="AP12" s="1"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="369" yWindow="876" count="48">
+  <dataValidations xWindow="369" yWindow="876" count="49">
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="Angle@VerticalAngle" prompt="Enter a valid value for this parameter." sqref="B3:B12"/>
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="Angle@HorizontalAngle" prompt="Enter a valid value for this parameter." sqref="C3:C12"/>
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="Horizontal@TopLeftDiagonal" prompt="Enter a valid value for this parameter." sqref="D3:D12"/>
@@ -2530,68 +2530,68 @@
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="Top@RatioRight" prompt="Enter a valid value for this parameter." sqref="P3:P12"/>
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="Bottom@RatioRight" prompt="Enter a valid value for this parameter." sqref="Q3:Q12"/>
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="Left@RatioBottom" prompt="Enter a valid value for this parameter." sqref="Z3:AO3 R3:R12"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="Right@RatioBottom" prompt="Enter a valid value for this parameter." sqref="S3:T12 U12"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConcaveEllipseBottomLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="V4:AO6 AF7:AF12">
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="Right@RatioBottom" prompt="Enter a valid value for this parameter." sqref="S3:S12 T3:T4 T12:U12"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConcaveEllipseBottomLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AF4:AF12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightConnectorBottom" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="V3 V7:V12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightConnectorBottom" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="V3:V12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightConnectorLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="W3 W7:W12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightConnectorLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="W3:W12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightConnectorRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="X3 X7:X12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightConnectorRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="X3:X12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightConnectorTop" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="Y3 Y7:Y12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightConnectorTop" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="Y3:Y12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@BoundingRatioBoxes" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AP3:AP12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightEdgeCornerTopLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="Z7:Z12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightEdgeCornerTopLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="Z4:Z12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightEdgeCornerTopRigh" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AA7:AA12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightEdgeCornerTopRigh" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AA4:AA12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightEdgeCornerBottomL" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AB7:AB12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightEdgeCornerBottomL" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AB4:AB12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightEdgeCornerBottomR" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AC7:AC12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@StraightEdgeCornerBottomR" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AC4:AC12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConcaveEllipseTopLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AD7:AD12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConcaveEllipseTopLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AD4:AD12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConcaveEllipseTopRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AE7:AE12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConcaveEllipseTopRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AE4:AE12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConcaveEllipseBottomRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AG7:AG12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConcaveEllipseBottomRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AG4:AG12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConvexEllipseTopLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AH7:AH12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConvexEllipseTopLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AH4:AH12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConvexEllipseTopRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AI7:AI12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConvexEllipseTopRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AI4:AI12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConvexEllipseBottomLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AJ7:AJ12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConvexEllipseBottomLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AJ4:AJ12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConvexEllipseBottomRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AK7:AK12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@ConvexEllipseBottomRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AK4:AK12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@DiagonalStraightTopLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AL7:AL12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@DiagonalStraightTopLeft" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AL4:AL12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@DiagonalStraightTopRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AM7:AM12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@DiagonalStraightTopRight" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AM4:AM12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@DiagonalStraightBottomLef" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AN7:AN12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@DiagonalStraightBottomLef" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AN4:AN12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@DiagonalStraightBottomRig" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AO7:AO12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@DiagonalStraightBottomRig" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="AO4:AO12">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$State@Notch" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="U3">
@@ -2621,6 +2621,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$State@Notch" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="U11">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="notch_depth@Notch" prompt="Enter a valid value for this parameter." sqref="T5:T11"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="AJ2" r:id="rId1"/>
@@ -2639,8 +2640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2676,7 +2677,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
@@ -2684,7 +2685,7 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="26" x14ac:dyDescent="0.6">

</xml_diff>